<commit_message>
Nokia challenge day 1
</commit_message>
<xml_diff>
--- a/out/production/Practice/Documents/Day_log_work.xlsx
+++ b/out/production/Practice/Documents/Day_log_work.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Practice\src\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24559CE5-E7A0-4E90-926D-1F15F409ECCA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4F76D72-442B-4892-8EBB-18A25BD0778C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1855" uniqueCount="790">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1927" uniqueCount="806">
   <si>
     <t>Ticket_id</t>
   </si>
@@ -2412,6 +2412,54 @@
   </si>
   <si>
     <t>y</t>
+  </si>
+  <si>
+    <t>keycloak upgrade to 6.0.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">es upgrade to 7.2.1 es started </t>
+  </si>
+  <si>
+    <t>es upgrade to 7.2.1 sg-config failing</t>
+  </si>
+  <si>
+    <t>spring  upgrade help to neeraj binder api fix</t>
+  </si>
+  <si>
+    <t>es upgrade search guard failed to come up reported to search guard</t>
+  </si>
+  <si>
+    <t>trying 7.3.0 version</t>
+  </si>
+  <si>
+    <t>temple: urukunda</t>
+  </si>
+  <si>
+    <t>4414;4092</t>
+  </si>
+  <si>
+    <t>kibana rpm build 5.6.15</t>
+  </si>
+  <si>
+    <t>lodash patch</t>
+  </si>
+  <si>
+    <t>lodash patch timelion removal</t>
+  </si>
+  <si>
+    <t>unit and integration test all modules</t>
+  </si>
+  <si>
+    <t>es fail with  class not found error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">search guard templates upgrade </t>
+  </si>
+  <si>
+    <t>es fixed by add correct jar then got sgadmin incomatible version problem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSL not loaded by ES </t>
   </si>
 </sst>
 </file>
@@ -11826,8 +11874,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEA16314-1EBD-45FC-BE59-12C57F1884F2}">
   <dimension ref="A1:R366"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A219" workbookViewId="0">
-      <selection activeCell="E236" sqref="E236"/>
+    <sheetView tabSelected="1" topLeftCell="A252" workbookViewId="0">
+      <selection activeCell="D267" sqref="D267"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -16844,8 +16892,11 @@
       <c r="O228" s="12"/>
     </row>
     <row r="229" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A229">
+        <v>4092</v>
+      </c>
       <c r="B229" t="s">
-        <v>625</v>
+        <v>611</v>
       </c>
       <c r="C229">
         <v>8</v>
@@ -16898,10 +16949,22 @@
       <c r="O231" s="12"/>
     </row>
     <row r="232" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A232">
+        <v>4092</v>
+      </c>
+      <c r="B232" t="s">
+        <v>611</v>
+      </c>
+      <c r="C232">
+        <v>8</v>
+      </c>
       <c r="D232" s="12">
         <v>43696</v>
       </c>
       <c r="E232"/>
+      <c r="F232" s="3" t="s">
+        <v>788</v>
+      </c>
       <c r="I232" s="3"/>
       <c r="J232" s="3"/>
       <c r="K232" s="12"/>
@@ -16911,10 +16974,19 @@
       <c r="O232" s="12"/>
     </row>
     <row r="233" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A233">
+        <v>4092</v>
+      </c>
+      <c r="B233" t="s">
+        <v>611</v>
+      </c>
       <c r="D233" s="12">
         <v>43697</v>
       </c>
       <c r="E233"/>
+      <c r="F233" s="3" t="s">
+        <v>788</v>
+      </c>
       <c r="I233" s="3"/>
       <c r="J233" s="3"/>
       <c r="K233" s="12"/>
@@ -16924,10 +16996,24 @@
       <c r="O233" s="12"/>
     </row>
     <row r="234" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A234">
+        <v>3978</v>
+      </c>
+      <c r="B234" t="s">
+        <v>611</v>
+      </c>
+      <c r="C234">
+        <v>8</v>
+      </c>
       <c r="D234" s="12">
         <v>43698</v>
       </c>
-      <c r="E234"/>
+      <c r="E234" t="s">
+        <v>787</v>
+      </c>
+      <c r="F234" s="3" t="s">
+        <v>790</v>
+      </c>
       <c r="I234" s="3"/>
       <c r="J234" s="3"/>
       <c r="K234" s="12"/>
@@ -16937,10 +17023,24 @@
       <c r="O234" s="12"/>
     </row>
     <row r="235" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A235">
+        <v>3978</v>
+      </c>
+      <c r="B235" t="s">
+        <v>611</v>
+      </c>
+      <c r="C235">
+        <v>8</v>
+      </c>
       <c r="D235" s="12">
         <v>43699</v>
       </c>
-      <c r="E235"/>
+      <c r="E235" t="s">
+        <v>787</v>
+      </c>
+      <c r="F235" s="3" t="s">
+        <v>790</v>
+      </c>
       <c r="I235" s="3"/>
       <c r="J235" s="3"/>
       <c r="K235" s="12"/>
@@ -16950,10 +17050,24 @@
       <c r="O235" s="12"/>
     </row>
     <row r="236" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A236">
+        <v>4092</v>
+      </c>
+      <c r="B236" t="s">
+        <v>611</v>
+      </c>
+      <c r="C236">
+        <v>8</v>
+      </c>
       <c r="D236" s="12">
         <v>43700</v>
       </c>
-      <c r="E236"/>
+      <c r="E236" t="s">
+        <v>787</v>
+      </c>
+      <c r="F236" s="3" t="s">
+        <v>788</v>
+      </c>
       <c r="I236" s="3"/>
       <c r="J236" s="3"/>
       <c r="K236" s="12"/>
@@ -16966,7 +17080,9 @@
       <c r="D237" s="12">
         <v>43701</v>
       </c>
-      <c r="E237"/>
+      <c r="E237" t="s">
+        <v>150</v>
+      </c>
       <c r="I237" s="3"/>
       <c r="J237" s="3"/>
       <c r="K237" s="12"/>
@@ -16979,7 +17095,9 @@
       <c r="D238" s="12">
         <v>43702</v>
       </c>
-      <c r="E238"/>
+      <c r="E238" t="s">
+        <v>150</v>
+      </c>
       <c r="I238" s="3"/>
       <c r="J238" s="3"/>
       <c r="K238" s="12"/>
@@ -16992,7 +17110,12 @@
       <c r="D239" s="12">
         <v>43703</v>
       </c>
-      <c r="E239"/>
+      <c r="E239" t="s">
+        <v>81</v>
+      </c>
+      <c r="F239" s="3" t="s">
+        <v>796</v>
+      </c>
       <c r="I239" s="3"/>
       <c r="J239" s="3"/>
       <c r="K239" s="12"/>
@@ -17002,10 +17125,24 @@
       <c r="O239" s="12"/>
     </row>
     <row r="240" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A240">
+        <v>4092</v>
+      </c>
+      <c r="B240" t="s">
+        <v>611</v>
+      </c>
+      <c r="C240">
+        <v>8</v>
+      </c>
       <c r="D240" s="12">
         <v>43704</v>
       </c>
-      <c r="E240"/>
+      <c r="E240" t="s">
+        <v>787</v>
+      </c>
+      <c r="F240" s="3" t="s">
+        <v>788</v>
+      </c>
       <c r="I240" s="3"/>
       <c r="J240" s="3"/>
       <c r="K240" s="12"/>
@@ -17015,10 +17152,24 @@
       <c r="O240" s="12"/>
     </row>
     <row r="241" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A241">
+        <v>4092</v>
+      </c>
+      <c r="B241" t="s">
+        <v>611</v>
+      </c>
+      <c r="C241">
+        <v>8</v>
+      </c>
       <c r="D241" s="12">
         <v>43705</v>
       </c>
-      <c r="E241"/>
+      <c r="E241" t="s">
+        <v>787</v>
+      </c>
+      <c r="F241" s="3" t="s">
+        <v>791</v>
+      </c>
       <c r="I241" s="3"/>
       <c r="J241" s="3"/>
       <c r="K241" s="12"/>
@@ -17028,10 +17179,24 @@
       <c r="O241" s="12"/>
     </row>
     <row r="242" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A242">
+        <v>4092</v>
+      </c>
+      <c r="B242" t="s">
+        <v>611</v>
+      </c>
+      <c r="C242">
+        <v>8</v>
+      </c>
       <c r="D242" s="12">
         <v>43706</v>
       </c>
-      <c r="E242"/>
+      <c r="E242" t="s">
+        <v>787</v>
+      </c>
+      <c r="F242" s="3" t="s">
+        <v>792</v>
+      </c>
       <c r="I242" s="3"/>
       <c r="J242" s="3"/>
       <c r="K242" s="12"/>
@@ -17041,10 +17206,24 @@
       <c r="O242" s="12"/>
     </row>
     <row r="243" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A243">
+        <v>4385</v>
+      </c>
+      <c r="B243" t="s">
+        <v>611</v>
+      </c>
+      <c r="C243">
+        <v>8</v>
+      </c>
       <c r="D243" s="12">
         <v>43707</v>
       </c>
-      <c r="E243"/>
+      <c r="E243" t="s">
+        <v>787</v>
+      </c>
+      <c r="F243" s="3" t="s">
+        <v>793</v>
+      </c>
       <c r="I243" s="3"/>
       <c r="J243" s="3"/>
       <c r="K243" s="12"/>
@@ -17057,7 +17236,9 @@
       <c r="D244" s="12">
         <v>43708</v>
       </c>
-      <c r="E244"/>
+      <c r="E244" t="s">
+        <v>150</v>
+      </c>
       <c r="I244" s="3"/>
       <c r="J244" s="3"/>
       <c r="K244" s="12"/>
@@ -17070,7 +17251,9 @@
       <c r="D245" s="12">
         <v>43709</v>
       </c>
-      <c r="E245"/>
+      <c r="E245" t="s">
+        <v>150</v>
+      </c>
       <c r="I245" s="3"/>
       <c r="J245" s="3"/>
       <c r="K245" s="12"/>
@@ -17097,11 +17280,25 @@
       <c r="N246" s="12"/>
       <c r="O246" s="12"/>
     </row>
-    <row r="247" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+      <c r="A247">
+        <v>4092</v>
+      </c>
+      <c r="B247" t="s">
+        <v>611</v>
+      </c>
+      <c r="C247">
+        <v>8</v>
+      </c>
       <c r="D247" s="12">
         <v>43711</v>
       </c>
-      <c r="E247"/>
+      <c r="E247" t="s">
+        <v>787</v>
+      </c>
+      <c r="F247" s="3" t="s">
+        <v>794</v>
+      </c>
       <c r="I247" s="3"/>
       <c r="J247" s="3"/>
       <c r="K247" s="12"/>
@@ -17111,10 +17308,24 @@
       <c r="O247" s="12"/>
     </row>
     <row r="248" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A248">
+        <v>4092</v>
+      </c>
+      <c r="B248" t="s">
+        <v>611</v>
+      </c>
+      <c r="C248">
+        <v>8</v>
+      </c>
       <c r="D248" s="12">
         <v>43712</v>
       </c>
-      <c r="E248"/>
+      <c r="E248" t="s">
+        <v>787</v>
+      </c>
+      <c r="F248" s="3" t="s">
+        <v>795</v>
+      </c>
       <c r="I248" s="3"/>
       <c r="J248" s="3"/>
       <c r="K248" s="12"/>
@@ -17124,10 +17335,22 @@
       <c r="O248" s="12"/>
     </row>
     <row r="249" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A249">
+        <v>4092</v>
+      </c>
+      <c r="B249" t="s">
+        <v>611</v>
+      </c>
+      <c r="C249">
+        <v>8</v>
+      </c>
       <c r="D249" s="12">
         <v>43713</v>
       </c>
       <c r="E249"/>
+      <c r="F249" s="3" t="s">
+        <v>802</v>
+      </c>
       <c r="I249" s="3"/>
       <c r="J249" s="3"/>
       <c r="K249" s="12"/>
@@ -17136,11 +17359,23 @@
       <c r="N249" s="12"/>
       <c r="O249" s="12"/>
     </row>
-    <row r="250" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+      <c r="A250">
+        <v>4092</v>
+      </c>
+      <c r="B250" t="s">
+        <v>611</v>
+      </c>
+      <c r="C250">
+        <v>8</v>
+      </c>
       <c r="D250" s="12">
         <v>43714</v>
       </c>
       <c r="E250"/>
+      <c r="F250" s="3" t="s">
+        <v>804</v>
+      </c>
       <c r="I250" s="3"/>
       <c r="J250" s="3"/>
       <c r="K250" s="12"/>
@@ -17153,7 +17388,9 @@
       <c r="D251" s="12">
         <v>43715</v>
       </c>
-      <c r="E251"/>
+      <c r="E251" t="s">
+        <v>150</v>
+      </c>
       <c r="I251" s="3"/>
       <c r="J251" s="3"/>
       <c r="K251" s="12"/>
@@ -17166,7 +17403,9 @@
       <c r="D252" s="12">
         <v>43716</v>
       </c>
-      <c r="E252"/>
+      <c r="E252" t="s">
+        <v>150</v>
+      </c>
       <c r="I252" s="3"/>
       <c r="J252" s="3"/>
       <c r="K252" s="12"/>
@@ -17176,10 +17415,22 @@
       <c r="O252" s="12"/>
     </row>
     <row r="253" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A253">
+        <v>4092</v>
+      </c>
+      <c r="B253" t="s">
+        <v>611</v>
+      </c>
+      <c r="C253">
+        <v>8</v>
+      </c>
       <c r="D253" s="12">
         <v>43717</v>
       </c>
       <c r="E253"/>
+      <c r="F253" s="3" t="s">
+        <v>803</v>
+      </c>
       <c r="I253" s="3"/>
       <c r="J253" s="3"/>
       <c r="K253" s="12"/>
@@ -17189,10 +17440,22 @@
       <c r="O253" s="12"/>
     </row>
     <row r="254" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A254">
+        <v>4092</v>
+      </c>
+      <c r="B254" t="s">
+        <v>611</v>
+      </c>
+      <c r="C254">
+        <v>8</v>
+      </c>
       <c r="D254" s="12">
         <v>43718</v>
       </c>
       <c r="E254"/>
+      <c r="F254" s="3" t="s">
+        <v>803</v>
+      </c>
       <c r="I254" s="3"/>
       <c r="J254" s="3"/>
       <c r="K254" s="12"/>
@@ -17202,10 +17465,22 @@
       <c r="O254" s="12"/>
     </row>
     <row r="255" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A255">
+        <v>4092</v>
+      </c>
+      <c r="B255" t="s">
+        <v>611</v>
+      </c>
+      <c r="C255">
+        <v>8</v>
+      </c>
       <c r="D255" s="12">
         <v>43719</v>
       </c>
       <c r="E255"/>
+      <c r="F255" s="3" t="s">
+        <v>803</v>
+      </c>
       <c r="I255" s="3"/>
       <c r="J255" s="3"/>
       <c r="K255" s="12"/>
@@ -17215,10 +17490,22 @@
       <c r="O255" s="12"/>
     </row>
     <row r="256" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A256">
+        <v>4092</v>
+      </c>
+      <c r="B256" t="s">
+        <v>611</v>
+      </c>
+      <c r="C256">
+        <v>8</v>
+      </c>
       <c r="D256" s="12">
         <v>43720</v>
       </c>
       <c r="E256"/>
+      <c r="F256" s="3" t="s">
+        <v>805</v>
+      </c>
       <c r="I256" s="3"/>
       <c r="J256" s="3"/>
       <c r="K256" s="12"/>
@@ -17227,11 +17514,23 @@
       <c r="N256" s="12"/>
       <c r="O256" s="12"/>
     </row>
-    <row r="257" spans="4:15" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A257">
+        <v>4092</v>
+      </c>
+      <c r="B257" t="s">
+        <v>611</v>
+      </c>
+      <c r="C257">
+        <v>8</v>
+      </c>
       <c r="D257" s="12">
         <v>43721</v>
       </c>
       <c r="E257"/>
+      <c r="F257" s="3" t="s">
+        <v>805</v>
+      </c>
       <c r="I257" s="3"/>
       <c r="J257" s="3"/>
       <c r="K257" s="12"/>
@@ -17240,11 +17539,13 @@
       <c r="N257" s="12"/>
       <c r="O257" s="12"/>
     </row>
-    <row r="258" spans="4:15" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:15" x14ac:dyDescent="0.35">
       <c r="D258" s="12">
         <v>43722</v>
       </c>
-      <c r="E258"/>
+      <c r="E258" t="s">
+        <v>150</v>
+      </c>
       <c r="I258" s="3"/>
       <c r="J258" s="3"/>
       <c r="K258" s="12"/>
@@ -17253,11 +17554,13 @@
       <c r="N258" s="12"/>
       <c r="O258" s="12"/>
     </row>
-    <row r="259" spans="4:15" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:15" x14ac:dyDescent="0.35">
       <c r="D259" s="12">
         <v>43723</v>
       </c>
-      <c r="E259"/>
+      <c r="E259" t="s">
+        <v>150</v>
+      </c>
       <c r="I259" s="3"/>
       <c r="J259" s="3"/>
       <c r="K259" s="12"/>
@@ -17266,11 +17569,23 @@
       <c r="N259" s="12"/>
       <c r="O259" s="12"/>
     </row>
-    <row r="260" spans="4:15" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A260" s="5" t="s">
+        <v>797</v>
+      </c>
+      <c r="B260" t="s">
+        <v>611</v>
+      </c>
+      <c r="C260">
+        <v>8</v>
+      </c>
       <c r="D260" s="12">
         <v>43724</v>
       </c>
       <c r="E260"/>
+      <c r="F260" s="3" t="s">
+        <v>798</v>
+      </c>
       <c r="I260" s="3"/>
       <c r="J260" s="3"/>
       <c r="K260" s="12"/>
@@ -17279,11 +17594,23 @@
       <c r="N260" s="12"/>
       <c r="O260" s="12"/>
     </row>
-    <row r="261" spans="4:15" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A261" s="5" t="s">
+        <v>797</v>
+      </c>
+      <c r="B261" t="s">
+        <v>611</v>
+      </c>
+      <c r="C261">
+        <v>8</v>
+      </c>
       <c r="D261" s="12">
         <v>43725</v>
       </c>
       <c r="E261"/>
+      <c r="F261" s="3" t="s">
+        <v>799</v>
+      </c>
       <c r="I261" s="3"/>
       <c r="J261" s="3"/>
       <c r="K261" s="12"/>
@@ -17292,11 +17619,23 @@
       <c r="N261" s="12"/>
       <c r="O261" s="12"/>
     </row>
-    <row r="262" spans="4:15" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A262" s="5" t="s">
+        <v>797</v>
+      </c>
+      <c r="B262" t="s">
+        <v>611</v>
+      </c>
+      <c r="C262">
+        <v>8</v>
+      </c>
       <c r="D262" s="12">
         <v>43726</v>
       </c>
       <c r="E262"/>
+      <c r="F262" s="3" t="s">
+        <v>799</v>
+      </c>
       <c r="I262" s="3"/>
       <c r="J262" s="3"/>
       <c r="K262" s="12"/>
@@ -17305,11 +17644,23 @@
       <c r="N262" s="12"/>
       <c r="O262" s="12"/>
     </row>
-    <row r="263" spans="4:15" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A263" s="5" t="s">
+        <v>797</v>
+      </c>
+      <c r="B263" t="s">
+        <v>611</v>
+      </c>
+      <c r="C263">
+        <v>8</v>
+      </c>
       <c r="D263" s="12">
         <v>43727</v>
       </c>
       <c r="E263"/>
+      <c r="F263" s="3" t="s">
+        <v>800</v>
+      </c>
       <c r="I263" s="3"/>
       <c r="J263" s="3"/>
       <c r="K263" s="12"/>
@@ -17318,11 +17669,23 @@
       <c r="N263" s="12"/>
       <c r="O263" s="12"/>
     </row>
-    <row r="264" spans="4:15" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A264" s="5" t="s">
+        <v>797</v>
+      </c>
+      <c r="B264" t="s">
+        <v>611</v>
+      </c>
+      <c r="C264">
+        <v>8</v>
+      </c>
       <c r="D264" s="12">
         <v>43728</v>
       </c>
       <c r="E264"/>
+      <c r="F264" s="3" t="s">
+        <v>801</v>
+      </c>
       <c r="I264" s="3"/>
       <c r="J264" s="3"/>
       <c r="K264" s="12"/>
@@ -17331,11 +17694,13 @@
       <c r="N264" s="12"/>
       <c r="O264" s="12"/>
     </row>
-    <row r="265" spans="4:15" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:15" x14ac:dyDescent="0.35">
       <c r="D265" s="12">
         <v>43729</v>
       </c>
-      <c r="E265"/>
+      <c r="E265" t="s">
+        <v>150</v>
+      </c>
       <c r="I265" s="3"/>
       <c r="J265" s="3"/>
       <c r="K265" s="12"/>
@@ -17344,11 +17709,13 @@
       <c r="N265" s="12"/>
       <c r="O265" s="12"/>
     </row>
-    <row r="266" spans="4:15" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:15" x14ac:dyDescent="0.35">
       <c r="D266" s="12">
         <v>43730</v>
       </c>
-      <c r="E266"/>
+      <c r="E266" t="s">
+        <v>150</v>
+      </c>
       <c r="I266" s="3"/>
       <c r="J266" s="3"/>
       <c r="K266" s="12"/>
@@ -17357,7 +17724,7 @@
       <c r="N266" s="12"/>
       <c r="O266" s="12"/>
     </row>
-    <row r="267" spans="4:15" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:15" x14ac:dyDescent="0.35">
       <c r="D267" s="12">
         <v>43731</v>
       </c>
@@ -17370,7 +17737,7 @@
       <c r="N267" s="12"/>
       <c r="O267" s="12"/>
     </row>
-    <row r="268" spans="4:15" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:15" x14ac:dyDescent="0.35">
       <c r="D268" s="12">
         <v>43732</v>
       </c>
@@ -17383,7 +17750,7 @@
       <c r="N268" s="12"/>
       <c r="O268" s="12"/>
     </row>
-    <row r="269" spans="4:15" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:15" x14ac:dyDescent="0.35">
       <c r="D269" s="12">
         <v>43733</v>
       </c>
@@ -17396,7 +17763,7 @@
       <c r="N269" s="12"/>
       <c r="O269" s="12"/>
     </row>
-    <row r="270" spans="4:15" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:15" x14ac:dyDescent="0.35">
       <c r="D270" s="12">
         <v>43734</v>
       </c>
@@ -17409,7 +17776,7 @@
       <c r="N270" s="12"/>
       <c r="O270" s="12"/>
     </row>
-    <row r="271" spans="4:15" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:15" x14ac:dyDescent="0.35">
       <c r="D271" s="12">
         <v>43735</v>
       </c>
@@ -17422,7 +17789,7 @@
       <c r="N271" s="12"/>
       <c r="O271" s="12"/>
     </row>
-    <row r="272" spans="4:15" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:15" x14ac:dyDescent="0.35">
       <c r="D272" s="12">
         <v>43736</v>
       </c>

</xml_diff>